<commit_message>
Update NCDC mapping and EMIF Twins
</commit_message>
<xml_diff>
--- a/ncdc_mappings/ncdc_minimal_dataset.xlsx
+++ b/ncdc_mappings/ncdc_minimal_dataset.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/OneDrive - Maastro - Clinic/Pedro Files/Data Harmonization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://maastro-my.sharepoint.com/personal/pedro_mateus_maastro_nl/Documents/Pedro Files/Data Harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B9D812-1676-8949-AC2D-08B3C8C8799F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{CFD7E28C-48FE-9D4B-9FBD-FF4601B5D85E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B515141-2EEF-564C-BDB5-8BB5993C00B8}"/>
   <bookViews>
     <workbookView xWindow="2960" yWindow="500" windowWidth="33600" windowHeight="19260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -366,7 +366,7 @@
     However, storing the information for 2 different times may be confusing. Probably the one that falls in the interval 20-30 minutes will be more suitable</t>
       </text>
     </comment>
-    <comment ref="D256" authorId="32" shapeId="0" xr:uid="{6A958D43-89AC-C443-90B2-E839939ED9BB}">
+    <comment ref="D257" authorId="32" shapeId="0" xr:uid="{6A958D43-89AC-C443-90B2-E839939ED9BB}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -374,7 +374,7 @@
     Generic concept only from SNOMED for the Boston Naming Test: 4164808</t>
       </text>
     </comment>
-    <comment ref="O280" authorId="33" shapeId="0" xr:uid="{C21DF866-3B02-8D43-BDB4-19473A2B92EE}">
+    <comment ref="O281" authorId="33" shapeId="0" xr:uid="{C21DF866-3B02-8D43-BDB4-19473A2B92EE}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -382,7 +382,7 @@
     Observation (SNOMED): 4136437</t>
       </text>
     </comment>
-    <comment ref="O281" authorId="34" shapeId="0" xr:uid="{6D0CD4A8-48D1-4246-9DC1-32FEBE702D51}">
+    <comment ref="O282" authorId="34" shapeId="0" xr:uid="{6D0CD4A8-48D1-4246-9DC1-32FEBE702D51}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -390,7 +390,7 @@
     Observation (SNOMED) 45768724</t>
       </text>
     </comment>
-    <comment ref="O282" authorId="35" shapeId="0" xr:uid="{B59C5FEF-8EFD-C648-A78A-AFBCA7EF7266}">
+    <comment ref="O283" authorId="35" shapeId="0" xr:uid="{B59C5FEF-8EFD-C648-A78A-AFBCA7EF7266}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -398,7 +398,7 @@
     Observation (SNOMED) 45768723</t>
       </text>
     </comment>
-    <comment ref="O284" authorId="36" shapeId="0" xr:uid="{BCD976E6-B6D9-D546-9016-DBD9D0F54E91}">
+    <comment ref="O285" authorId="36" shapeId="0" xr:uid="{BCD976E6-B6D9-D546-9016-DBD9D0F54E91}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -406,7 +406,7 @@
     Observation (SNOMED) 4079321</t>
       </text>
     </comment>
-    <comment ref="O285" authorId="37" shapeId="0" xr:uid="{DFA827BB-C401-AD42-9C05-074FE05BA8AF}">
+    <comment ref="O286" authorId="37" shapeId="0" xr:uid="{DFA827BB-C401-AD42-9C05-074FE05BA8AF}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -416,7 +416,7 @@
     4299446</t>
       </text>
     </comment>
-    <comment ref="O286" authorId="38" shapeId="0" xr:uid="{8B270D9A-52A2-8745-B447-8EF3342DED56}">
+    <comment ref="O287" authorId="38" shapeId="0" xr:uid="{8B270D9A-52A2-8745-B447-8EF3342DED56}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -424,7 +424,7 @@
     Observation (SNOMED) 4012274</t>
       </text>
     </comment>
-    <comment ref="O287" authorId="39" shapeId="0" xr:uid="{48DC908A-650A-A142-B529-8C8185B7B723}">
+    <comment ref="O288" authorId="39" shapeId="0" xr:uid="{48DC908A-650A-A142-B529-8C8185B7B723}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -435,7 +435,7 @@
     Observation (SNOMED) - 4221816 (referes to the component itself)</t>
       </text>
     </comment>
-    <comment ref="D293" authorId="40" shapeId="0" xr:uid="{70609BE4-D9A6-3145-A3F3-5832E54D4EE2}">
+    <comment ref="D294" authorId="40" shapeId="0" xr:uid="{70609BE4-D9A6-3145-A3F3-5832E54D4EE2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -700,7 +700,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4573" uniqueCount="957">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4580" uniqueCount="958">
   <si>
     <t>Main category</t>
   </si>
@@ -3531,12 +3531,6 @@
     <t>VOSP number location</t>
   </si>
   <si>
-    <t>Priority_executive_wais_3</t>
-  </si>
-  <si>
-    <t>WAIS-III digit span forward and backward</t>
-  </si>
-  <si>
     <t>Priority_language_cantab</t>
   </si>
   <si>
@@ -3595,9 +3589,6 @@
   </si>
   <si>
     <t>HADS</t>
-  </si>
-  <si>
-    <t>Meaasurement</t>
   </si>
   <si>
     <t>Cardiovascular_disease</t>
@@ -3617,6 +3608,18 @@
   </si>
   <si>
     <t>hdl_ratio</t>
+  </si>
+  <si>
+    <t>Priority_executive_wais_3_b</t>
+  </si>
+  <si>
+    <t>Priority_executive_wais_3_f</t>
+  </si>
+  <si>
+    <t>WAIS-III digit span backward</t>
+  </si>
+  <si>
+    <t>WAIS-III digit span forward</t>
   </si>
 </sst>
 </file>
@@ -5788,38 +5791,38 @@
   <threadedComment ref="D218" dT="2021-07-19T16:04:57.29" personId="{D0C6A6B3-9E49-B948-BD43-8E6E77C05370}" id="{75CAA762-6AD4-934F-A0AD-B9AFDD6D31E9}" parentId="{7B408D37-7963-244B-BBC8-4A2BD19C9A8C}">
     <text>However, storing the information for 2 different times may be confusing. Probably the one that falls in the interval 20-30 minutes will be more suitable</text>
   </threadedComment>
-  <threadedComment ref="D256" dT="2021-07-08T14:57:23.15" personId="{D0C6A6B3-9E49-B948-BD43-8E6E77C05370}" id="{6A958D43-89AC-C443-90B2-E839939ED9BB}">
+  <threadedComment ref="D257" dT="2021-07-08T14:57:23.15" personId="{D0C6A6B3-9E49-B948-BD43-8E6E77C05370}" id="{6A958D43-89AC-C443-90B2-E839939ED9BB}">
     <text>Generic concept only from SNOMED for the Boston Naming Test: 4164808</text>
   </threadedComment>
-  <threadedComment ref="O280" dT="2021-10-27T15:56:51.26" personId="{D0C6A6B3-9E49-B948-BD43-8E6E77C05370}" id="{C21DF866-3B02-8D43-BDB4-19473A2B92EE}">
+  <threadedComment ref="O281" dT="2021-10-27T15:56:51.26" personId="{D0C6A6B3-9E49-B948-BD43-8E6E77C05370}" id="{C21DF866-3B02-8D43-BDB4-19473A2B92EE}">
     <text>Observation (SNOMED): 4136437</text>
   </threadedComment>
-  <threadedComment ref="O281" dT="2021-10-27T15:57:10.76" personId="{D0C6A6B3-9E49-B948-BD43-8E6E77C05370}" id="{6D0CD4A8-48D1-4246-9DC1-32FEBE702D51}">
+  <threadedComment ref="O282" dT="2021-10-27T15:57:10.76" personId="{D0C6A6B3-9E49-B948-BD43-8E6E77C05370}" id="{6D0CD4A8-48D1-4246-9DC1-32FEBE702D51}">
     <text>Observation (SNOMED) 45768724</text>
   </threadedComment>
-  <threadedComment ref="O282" dT="2021-10-27T15:59:18.03" personId="{D0C6A6B3-9E49-B948-BD43-8E6E77C05370}" id="{B59C5FEF-8EFD-C648-A78A-AFBCA7EF7266}">
+  <threadedComment ref="O283" dT="2021-10-27T15:59:18.03" personId="{D0C6A6B3-9E49-B948-BD43-8E6E77C05370}" id="{B59C5FEF-8EFD-C648-A78A-AFBCA7EF7266}">
     <text>Observation (SNOMED) 45768723</text>
   </threadedComment>
-  <threadedComment ref="O284" dT="2021-10-27T16:01:02.13" personId="{D0C6A6B3-9E49-B948-BD43-8E6E77C05370}" id="{BCD976E6-B6D9-D546-9016-DBD9D0F54E91}">
+  <threadedComment ref="O285" dT="2021-10-27T16:01:02.13" personId="{D0C6A6B3-9E49-B948-BD43-8E6E77C05370}" id="{BCD976E6-B6D9-D546-9016-DBD9D0F54E91}">
     <text>Observation (SNOMED) 4079321</text>
   </threadedComment>
-  <threadedComment ref="O285" dT="2021-07-02T12:24:20.39" personId="{98691CDF-5915-8B45-A1D3-22E1ADD8314B}" id="{DFA827BB-C401-AD42-9C05-074FE05BA8AF}">
+  <threadedComment ref="O286" dT="2021-07-02T12:24:20.39" personId="{98691CDF-5915-8B45-A1D3-22E1ADD8314B}" id="{DFA827BB-C401-AD42-9C05-074FE05BA8AF}">
     <text>Matches to “Neurofilament protein” - no clear match to NFL, maybe a new concept or the link to the ontology can be enough?</text>
   </threadedComment>
-  <threadedComment ref="O285" dT="2021-10-27T16:04:29.90" personId="{D0C6A6B3-9E49-B948-BD43-8E6E77C05370}" id="{236EE8B4-0B5A-B546-910E-201CC41AB22E}" parentId="{DFA827BB-C401-AD42-9C05-074FE05BA8AF}">
+  <threadedComment ref="O286" dT="2021-10-27T16:04:29.90" personId="{D0C6A6B3-9E49-B948-BD43-8E6E77C05370}" id="{236EE8B4-0B5A-B546-910E-201CC41AB22E}" parentId="{DFA827BB-C401-AD42-9C05-074FE05BA8AF}">
     <text>4299446</text>
   </threadedComment>
-  <threadedComment ref="O286" dT="2021-10-27T16:05:33.61" personId="{D0C6A6B3-9E49-B948-BD43-8E6E77C05370}" id="{8B270D9A-52A2-8745-B447-8EF3342DED56}">
+  <threadedComment ref="O287" dT="2021-10-27T16:05:33.61" personId="{D0C6A6B3-9E49-B948-BD43-8E6E77C05370}" id="{8B270D9A-52A2-8745-B447-8EF3342DED56}">
     <text>Observation (SNOMED) 4012274</text>
   </threadedComment>
-  <threadedComment ref="O287" dT="2021-10-27T16:07:09.40" personId="{D0C6A6B3-9E49-B948-BD43-8E6E77C05370}" id="{48DC908A-650A-A142-B529-8C8185B7B723}">
+  <threadedComment ref="O288" dT="2021-10-27T16:07:09.40" personId="{D0C6A6B3-9E49-B948-BD43-8E6E77C05370}" id="{48DC908A-650A-A142-B529-8C8185B7B723}">
     <text>Measurement meaning - Measurement of concentration of amyloid A in serum specimen (procedure)
 Serum amyloid A concentratio</text>
   </threadedComment>
-  <threadedComment ref="O287" dT="2021-10-27T16:07:50.16" personId="{D0C6A6B3-9E49-B948-BD43-8E6E77C05370}" id="{475E4E61-9156-CF48-A078-B50A8EE3149D}" parentId="{48DC908A-650A-A142-B529-8C8185B7B723}">
+  <threadedComment ref="O288" dT="2021-10-27T16:07:50.16" personId="{D0C6A6B3-9E49-B948-BD43-8E6E77C05370}" id="{475E4E61-9156-CF48-A078-B50A8EE3149D}" parentId="{48DC908A-650A-A142-B529-8C8185B7B723}">
     <text>Observation (SNOMED) - 4221816 (referes to the component itself)</text>
   </threadedComment>
-  <threadedComment ref="D293" dT="2021-07-02T12:47:45.50" personId="{98691CDF-5915-8B45-A1D3-22E1ADD8314B}" id="{70609BE4-D9A6-3145-A3F3-5832E54D4EE2}">
+  <threadedComment ref="D294" dT="2021-07-02T12:47:45.50" personId="{98691CDF-5915-8B45-A1D3-22E1ADD8314B}" id="{70609BE4-D9A6-3145-A3F3-5832E54D4EE2}">
     <text>All these fields require more information. Probably they represent measurements but more complete information is required to clearly identify what’s being measured/how and the units.</text>
   </threadedComment>
 </ThreadedComments>
@@ -5927,11 +5930,11 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:Y1266"/>
+  <dimension ref="A1:Y1267"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="89" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E95" sqref="E95"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="89" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A222" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O248" sqref="O248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="17"/>
@@ -9421,10 +9424,10 @@
       </c>
       <c r="C72" s="15"/>
       <c r="D72" s="15" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
       <c r="E72" s="16" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
       <c r="F72" s="15" t="s">
         <v>55</v>
@@ -9443,7 +9446,7 @@
         <v>337</v>
       </c>
       <c r="L72" s="16" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
       <c r="M72" s="27" t="s">
         <v>367</v>
@@ -10583,10 +10586,10 @@
       </c>
       <c r="C93" s="15"/>
       <c r="D93" s="15" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
       <c r="E93" s="16" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
       <c r="F93" s="15" t="s">
         <v>197</v>
@@ -12978,13 +12981,13 @@
       <c r="A141" s="59"/>
       <c r="B141" s="72"/>
       <c r="C141" s="27" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="D141" s="83" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="E141" s="87" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="F141" s="27" t="s">
         <v>309</v>
@@ -13002,7 +13005,7 @@
       </c>
       <c r="L141" s="16"/>
       <c r="M141" s="47" t="s">
-        <v>951</v>
+        <v>374</v>
       </c>
       <c r="N141" s="65" t="s">
         <v>368</v>
@@ -13029,13 +13032,13 @@
       <c r="A142" s="59"/>
       <c r="B142" s="72"/>
       <c r="C142" s="27" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="D142" s="83" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="E142" s="87" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="F142" s="27" t="s">
         <v>309</v>
@@ -13053,7 +13056,7 @@
       </c>
       <c r="L142" s="16"/>
       <c r="M142" s="47" t="s">
-        <v>951</v>
+        <v>374</v>
       </c>
       <c r="N142" s="65" t="s">
         <v>368</v>
@@ -17870,10 +17873,10 @@
       <c r="B246" s="67"/>
       <c r="C246" s="45"/>
       <c r="D246" s="84" t="s">
-        <v>929</v>
+        <v>954</v>
       </c>
       <c r="E246" s="84" t="s">
-        <v>930</v>
+        <v>956</v>
       </c>
       <c r="F246" s="27" t="s">
         <v>197</v>
@@ -17913,30 +17916,35 @@
       <c r="A247" s="59"/>
       <c r="B247" s="67"/>
       <c r="C247" s="45"/>
-      <c r="D247" s="77" t="s">
-        <v>521</v>
-      </c>
-      <c r="E247" s="76" t="s">
-        <v>519</v>
+      <c r="D247" s="84" t="s">
+        <v>955</v>
+      </c>
+      <c r="E247" s="84" t="s">
+        <v>957</v>
       </c>
       <c r="F247" s="27" t="s">
         <v>197</v>
       </c>
       <c r="G247" s="16"/>
-      <c r="H247" s="38"/>
-      <c r="I247" s="38"/>
+      <c r="H247" s="104" t="s">
+        <v>762</v>
+      </c>
+      <c r="I247" s="38" t="s">
+        <v>715</v>
+      </c>
       <c r="J247" s="15"/>
       <c r="K247" s="27" t="s">
         <v>337</v>
       </c>
       <c r="L247" s="27"/>
-      <c r="M247" s="27"/>
+      <c r="M247" s="27" t="s">
+        <v>374</v>
+      </c>
       <c r="N247" s="27"/>
-      <c r="O247" s="89"/>
-      <c r="P247" s="28" t="str">
-        <f t="shared" ref="P247:P264" si="18">IF(N247&lt;&gt;"",HYPERLINK(CONCATENATE("https:;;athena.ohdsi.org;search-terms;terms;",O247), CONCATENATE("Athena-",O247)),"")</f>
-        <v/>
-      </c>
+      <c r="O247" s="89">
+        <v>2000000134</v>
+      </c>
+      <c r="P247" s="28"/>
       <c r="Q247" s="27"/>
       <c r="R247" s="27"/>
       <c r="S247" s="27"/>
@@ -17948,38 +17956,30 @@
         <v>780</v>
       </c>
     </row>
-    <row r="248" spans="1:24" s="54" customFormat="1" ht="47" customHeight="1">
+    <row r="248" spans="1:24" s="54" customFormat="1" ht="16" customHeight="1">
       <c r="A248" s="59"/>
-      <c r="B248" s="67" t="s">
-        <v>150</v>
-      </c>
-      <c r="C248" s="27" t="s">
-        <v>136</v>
-      </c>
-      <c r="D248" s="27" t="s">
-        <v>209</v>
-      </c>
-      <c r="E248" s="45" t="s">
-        <v>251</v>
+      <c r="B248" s="67"/>
+      <c r="C248" s="45"/>
+      <c r="D248" s="77"/>
+      <c r="E248" s="76" t="s">
+        <v>519</v>
       </c>
       <c r="F248" s="27" t="s">
         <v>197</v>
       </c>
-      <c r="G248" s="15"/>
-      <c r="H248" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="I248" s="28"/>
+      <c r="G248" s="16"/>
+      <c r="H248" s="38"/>
+      <c r="I248" s="38"/>
       <c r="J248" s="15"/>
       <c r="K248" s="27" t="s">
         <v>337</v>
       </c>
-      <c r="L248" s="16"/>
+      <c r="L248" s="27"/>
       <c r="M248" s="27"/>
       <c r="N248" s="27"/>
-      <c r="O248" s="27"/>
+      <c r="O248" s="89"/>
       <c r="P248" s="28" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="P248:P265" si="18">IF(N248&lt;&gt;"",HYPERLINK(CONCATENATE("https:;;athena.ohdsi.org;search-terms;terms;",O248), CONCATENATE("Athena-",O248)),"")</f>
         <v/>
       </c>
       <c r="Q248" s="27"/>
@@ -17993,28 +17993,28 @@
         <v>780</v>
       </c>
     </row>
-    <row r="249" spans="1:24" s="54" customFormat="1" ht="16">
+    <row r="249" spans="1:24" s="54" customFormat="1" ht="47" customHeight="1">
       <c r="A249" s="59"/>
       <c r="B249" s="67" t="s">
         <v>150</v>
       </c>
       <c r="C249" s="27" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D249" s="27" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E249" s="45" t="s">
-        <v>133</v>
+        <v>251</v>
       </c>
       <c r="F249" s="27" t="s">
         <v>197</v>
       </c>
       <c r="G249" s="15"/>
-      <c r="H249" s="36" t="s">
-        <v>138</v>
-      </c>
-      <c r="I249" s="36"/>
+      <c r="H249" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="I249" s="28"/>
       <c r="J249" s="15"/>
       <c r="K249" s="27" t="s">
         <v>337</v>
@@ -18038,37 +18038,33 @@
         <v>780</v>
       </c>
     </row>
-    <row r="250" spans="1:24" s="54" customFormat="1" ht="110" customHeight="1">
+    <row r="250" spans="1:24" s="54" customFormat="1" ht="16">
       <c r="A250" s="59"/>
       <c r="B250" s="67" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C250" s="27" t="s">
-        <v>140</v>
-      </c>
-      <c r="D250" s="76" t="s">
-        <v>214</v>
-      </c>
-      <c r="E250" s="76" t="s">
-        <v>528</v>
+        <v>135</v>
+      </c>
+      <c r="D250" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="E250" s="45" t="s">
+        <v>133</v>
       </c>
       <c r="F250" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="G250" s="15" t="s">
-        <v>693</v>
-      </c>
-      <c r="H250" s="43" t="s">
-        <v>327</v>
-      </c>
-      <c r="I250" s="43"/>
+        <v>197</v>
+      </c>
+      <c r="G250" s="15"/>
+      <c r="H250" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="I250" s="36"/>
       <c r="J250" s="15"/>
       <c r="K250" s="27" t="s">
         <v>337</v>
       </c>
-      <c r="L250" s="16" t="s">
-        <v>694</v>
-      </c>
+      <c r="L250" s="16"/>
       <c r="M250" s="27"/>
       <c r="N250" s="27"/>
       <c r="O250" s="27"/>
@@ -18084,43 +18080,43 @@
       <c r="V250" s="27"/>
       <c r="W250" s="27"/>
       <c r="X250" s="15" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="251" spans="1:24" s="54" customFormat="1" ht="16" customHeight="1">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="251" spans="1:24" s="54" customFormat="1" ht="110" customHeight="1">
       <c r="A251" s="59"/>
-      <c r="B251" s="67"/>
-      <c r="C251" s="45" t="s">
-        <v>573</v>
-      </c>
-      <c r="D251" s="84" t="s">
-        <v>914</v>
-      </c>
-      <c r="E251" s="83" t="s">
-        <v>883</v>
+      <c r="B251" s="67" t="s">
+        <v>151</v>
+      </c>
+      <c r="C251" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="D251" s="76" t="s">
+        <v>214</v>
+      </c>
+      <c r="E251" s="76" t="s">
+        <v>528</v>
       </c>
       <c r="F251" s="27" t="s">
-        <v>197</v>
-      </c>
-      <c r="G251" s="16"/>
-      <c r="H251" s="104" t="s">
-        <v>762</v>
-      </c>
-      <c r="I251" s="28" t="s">
-        <v>715</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="G251" s="15" t="s">
+        <v>693</v>
+      </c>
+      <c r="H251" s="43" t="s">
+        <v>327</v>
+      </c>
+      <c r="I251" s="43"/>
       <c r="J251" s="15"/>
       <c r="K251" s="27" t="s">
         <v>337</v>
       </c>
-      <c r="L251" s="27"/>
-      <c r="M251" s="47" t="s">
-        <v>374</v>
-      </c>
+      <c r="L251" s="16" t="s">
+        <v>694</v>
+      </c>
+      <c r="M251" s="27"/>
       <c r="N251" s="27"/>
-      <c r="O251" s="89">
-        <v>2000000068</v>
-      </c>
+      <c r="O251" s="27"/>
       <c r="P251" s="28" t="str">
         <f t="shared" si="18"/>
         <v/>
@@ -18139,12 +18135,14 @@
     <row r="252" spans="1:24" s="54" customFormat="1" ht="16" customHeight="1">
       <c r="A252" s="59"/>
       <c r="B252" s="67"/>
-      <c r="C252" s="106"/>
+      <c r="C252" s="45" t="s">
+        <v>573</v>
+      </c>
       <c r="D252" s="84" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="E252" s="83" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="F252" s="27" t="s">
         <v>197</v>
@@ -18166,10 +18164,10 @@
       </c>
       <c r="N252" s="27"/>
       <c r="O252" s="89">
-        <v>2000000123</v>
+        <v>2000000068</v>
       </c>
       <c r="P252" s="28" t="str">
-        <f t="shared" ref="P252" si="19">IF(N252&lt;&gt;"",HYPERLINK(CONCATENATE("https:;;athena.ohdsi.org;search-terms;terms;",O252), CONCATENATE("Athena-",O252)),"")</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="Q252" s="27"/>
@@ -18186,11 +18184,12 @@
     <row r="253" spans="1:24" s="54" customFormat="1" ht="16" customHeight="1">
       <c r="A253" s="59"/>
       <c r="B253" s="67"/>
+      <c r="C253" s="106"/>
       <c r="D253" s="84" t="s">
-        <v>919</v>
-      </c>
-      <c r="E253" s="84" t="s">
-        <v>530</v>
+        <v>915</v>
+      </c>
+      <c r="E253" s="83" t="s">
+        <v>882</v>
       </c>
       <c r="F253" s="27" t="s">
         <v>197</v>
@@ -18212,10 +18211,10 @@
       </c>
       <c r="N253" s="27"/>
       <c r="O253" s="89">
-        <v>2000000069</v>
+        <v>2000000123</v>
       </c>
       <c r="P253" s="28" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="P253" si="19">IF(N253&lt;&gt;"",HYPERLINK(CONCATENATE("https:;;athena.ohdsi.org;search-terms;terms;",O253), CONCATENATE("Athena-",O253)),"")</f>
         <v/>
       </c>
       <c r="Q253" s="27"/>
@@ -18232,14 +18231,11 @@
     <row r="254" spans="1:24" s="54" customFormat="1" ht="16" customHeight="1">
       <c r="A254" s="59"/>
       <c r="B254" s="67"/>
-      <c r="C254" s="45" t="s">
-        <v>574</v>
-      </c>
       <c r="D254" s="84" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
       <c r="E254" s="84" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="F254" s="27" t="s">
         <v>197</v>
@@ -18261,7 +18257,7 @@
       </c>
       <c r="N254" s="27"/>
       <c r="O254" s="89">
-        <v>2000000070</v>
+        <v>2000000069</v>
       </c>
       <c r="P254" s="28" t="str">
         <f t="shared" si="18"/>
@@ -18281,12 +18277,14 @@
     <row r="255" spans="1:24" s="54" customFormat="1" ht="16" customHeight="1">
       <c r="A255" s="59"/>
       <c r="B255" s="67"/>
-      <c r="C255" s="45"/>
+      <c r="C255" s="45" t="s">
+        <v>574</v>
+      </c>
       <c r="D255" s="84" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="E255" s="84" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="F255" s="27" t="s">
         <v>197</v>
@@ -18308,7 +18306,7 @@
       </c>
       <c r="N255" s="27"/>
       <c r="O255" s="89">
-        <v>2000000071</v>
+        <v>2000000070</v>
       </c>
       <c r="P255" s="28" t="str">
         <f t="shared" si="18"/>
@@ -18328,14 +18326,12 @@
     <row r="256" spans="1:24" s="54" customFormat="1" ht="16" customHeight="1">
       <c r="A256" s="59"/>
       <c r="B256" s="67"/>
-      <c r="C256" s="45" t="s">
-        <v>581</v>
-      </c>
-      <c r="D256" s="83" t="s">
-        <v>575</v>
-      </c>
-      <c r="E256" s="83" t="s">
-        <v>578</v>
+      <c r="C256" s="45"/>
+      <c r="D256" s="84" t="s">
+        <v>918</v>
+      </c>
+      <c r="E256" s="84" t="s">
+        <v>532</v>
       </c>
       <c r="F256" s="27" t="s">
         <v>197</v>
@@ -18357,7 +18353,7 @@
       </c>
       <c r="N256" s="27"/>
       <c r="O256" s="89">
-        <v>2000000072</v>
+        <v>2000000071</v>
       </c>
       <c r="P256" s="28" t="str">
         <f t="shared" si="18"/>
@@ -18378,13 +18374,13 @@
       <c r="A257" s="59"/>
       <c r="B257" s="67"/>
       <c r="C257" s="45" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D257" s="83" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="E257" s="83" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F257" s="27" t="s">
         <v>197</v>
@@ -18406,7 +18402,7 @@
       </c>
       <c r="N257" s="27"/>
       <c r="O257" s="89">
-        <v>2000000073</v>
+        <v>2000000072</v>
       </c>
       <c r="P257" s="28" t="str">
         <f t="shared" si="18"/>
@@ -18427,13 +18423,13 @@
       <c r="A258" s="59"/>
       <c r="B258" s="67"/>
       <c r="C258" s="45" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D258" s="83" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E258" s="83" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="F258" s="27" t="s">
         <v>197</v>
@@ -18455,7 +18451,7 @@
       </c>
       <c r="N258" s="27"/>
       <c r="O258" s="89">
-        <v>2000000074</v>
+        <v>2000000073</v>
       </c>
       <c r="P258" s="28" t="str">
         <f t="shared" si="18"/>
@@ -18475,12 +18471,14 @@
     <row r="259" spans="1:24" s="54" customFormat="1" ht="16" customHeight="1">
       <c r="A259" s="59"/>
       <c r="B259" s="67"/>
-      <c r="C259" s="45"/>
+      <c r="C259" s="45" t="s">
+        <v>583</v>
+      </c>
       <c r="D259" s="83" t="s">
-        <v>526</v>
-      </c>
-      <c r="E259" s="84" t="s">
-        <v>739</v>
+        <v>577</v>
+      </c>
+      <c r="E259" s="83" t="s">
+        <v>580</v>
       </c>
       <c r="F259" s="27" t="s">
         <v>197</v>
@@ -18502,10 +18500,10 @@
       </c>
       <c r="N259" s="27"/>
       <c r="O259" s="89">
-        <v>2000000075</v>
+        <v>2000000074</v>
       </c>
       <c r="P259" s="28" t="str">
-        <f t="shared" ref="P259" si="20">IF(N259&lt;&gt;"",HYPERLINK(CONCATENATE("https:;;athena.ohdsi.org;search-terms;terms;",O259), CONCATENATE("Athena-",O259)),"")</f>
+        <f t="shared" si="18"/>
         <v/>
       </c>
       <c r="Q259" s="27"/>
@@ -18524,10 +18522,10 @@
       <c r="B260" s="67"/>
       <c r="C260" s="45"/>
       <c r="D260" s="83" t="s">
-        <v>916</v>
+        <v>526</v>
       </c>
       <c r="E260" s="84" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="F260" s="27" t="s">
         <v>197</v>
@@ -18549,10 +18547,10 @@
       </c>
       <c r="N260" s="27"/>
       <c r="O260" s="89">
-        <v>2000000086</v>
+        <v>2000000075</v>
       </c>
       <c r="P260" s="28" t="str">
-        <f t="shared" ref="P260" si="21">IF(N260&lt;&gt;"",HYPERLINK(CONCATENATE("https:;;athena.ohdsi.org;search-terms;terms;",O260), CONCATENATE("Athena-",O260)),"")</f>
+        <f t="shared" ref="P260" si="20">IF(N260&lt;&gt;"",HYPERLINK(CONCATENATE("https:;;athena.ohdsi.org;search-terms;terms;",O260), CONCATENATE("Athena-",O260)),"")</f>
         <v/>
       </c>
       <c r="Q260" s="27"/>
@@ -18571,10 +18569,10 @@
       <c r="B261" s="67"/>
       <c r="C261" s="45"/>
       <c r="D261" s="83" t="s">
-        <v>931</v>
+        <v>916</v>
       </c>
       <c r="E261" s="84" t="s">
-        <v>932</v>
+        <v>740</v>
       </c>
       <c r="F261" s="27" t="s">
         <v>197</v>
@@ -18596,9 +18594,12 @@
       </c>
       <c r="N261" s="27"/>
       <c r="O261" s="89">
-        <v>2000000129</v>
-      </c>
-      <c r="P261" s="28"/>
+        <v>2000000086</v>
+      </c>
+      <c r="P261" s="28" t="str">
+        <f t="shared" ref="P261" si="21">IF(N261&lt;&gt;"",HYPERLINK(CONCATENATE("https:;;athena.ohdsi.org;search-terms;terms;",O261), CONCATENATE("Athena-",O261)),"")</f>
+        <v/>
+      </c>
       <c r="Q261" s="27"/>
       <c r="R261" s="27"/>
       <c r="S261" s="27"/>
@@ -18614,11 +18615,11 @@
       <c r="A262" s="59"/>
       <c r="B262" s="67"/>
       <c r="C262" s="45"/>
-      <c r="D262" s="76" t="s">
-        <v>527</v>
-      </c>
-      <c r="E262" s="77" t="s">
-        <v>529</v>
+      <c r="D262" s="83" t="s">
+        <v>929</v>
+      </c>
+      <c r="E262" s="84" t="s">
+        <v>930</v>
       </c>
       <c r="F262" s="27" t="s">
         <v>197</v>
@@ -18627,19 +18628,22 @@
       <c r="H262" s="104" t="s">
         <v>762</v>
       </c>
-      <c r="I262" s="28"/>
+      <c r="I262" s="28" t="s">
+        <v>715</v>
+      </c>
       <c r="J262" s="15"/>
       <c r="K262" s="27" t="s">
         <v>337</v>
       </c>
       <c r="L262" s="27"/>
-      <c r="M262" s="47"/>
+      <c r="M262" s="47" t="s">
+        <v>374</v>
+      </c>
       <c r="N262" s="27"/>
-      <c r="O262" s="89"/>
-      <c r="P262" s="28" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
+      <c r="O262" s="89">
+        <v>2000000129</v>
+      </c>
+      <c r="P262" s="28"/>
       <c r="Q262" s="27"/>
       <c r="R262" s="27"/>
       <c r="S262" s="27"/>
@@ -18651,24 +18655,20 @@
         <v>776</v>
       </c>
     </row>
-    <row r="263" spans="1:24" s="54" customFormat="1" ht="44" customHeight="1">
+    <row r="263" spans="1:24" s="54" customFormat="1" ht="16" customHeight="1">
       <c r="A263" s="59"/>
-      <c r="B263" s="67" t="s">
-        <v>151</v>
-      </c>
-      <c r="C263" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="D263" s="27" t="s">
-        <v>212</v>
-      </c>
-      <c r="E263" s="45" t="s">
-        <v>130</v>
+      <c r="B263" s="67"/>
+      <c r="C263" s="45"/>
+      <c r="D263" s="76" t="s">
+        <v>527</v>
+      </c>
+      <c r="E263" s="77" t="s">
+        <v>529</v>
       </c>
       <c r="F263" s="27" t="s">
         <v>197</v>
       </c>
-      <c r="G263" s="15"/>
+      <c r="G263" s="16"/>
       <c r="H263" s="104" t="s">
         <v>762</v>
       </c>
@@ -18677,10 +18677,10 @@
       <c r="K263" s="27" t="s">
         <v>337</v>
       </c>
-      <c r="L263" s="16"/>
-      <c r="M263" s="27"/>
+      <c r="L263" s="27"/>
+      <c r="M263" s="47"/>
       <c r="N263" s="27"/>
-      <c r="O263" s="27"/>
+      <c r="O263" s="89"/>
       <c r="P263" s="28" t="str">
         <f t="shared" si="18"/>
         <v/>
@@ -18696,33 +18696,33 @@
         <v>776</v>
       </c>
     </row>
-    <row r="264" spans="1:24" s="54" customFormat="1" ht="15">
+    <row r="264" spans="1:24" s="54" customFormat="1" ht="44" customHeight="1">
       <c r="A264" s="59"/>
-      <c r="B264" s="49" t="s">
+      <c r="B264" s="67" t="s">
         <v>151</v>
       </c>
-      <c r="C264" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="D264" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="E264" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="F264" s="15" t="s">
+      <c r="C264" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="D264" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="E264" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="F264" s="27" t="s">
         <v>197</v>
       </c>
       <c r="G264" s="15"/>
-      <c r="H264" s="36" t="s">
-        <v>138</v>
-      </c>
-      <c r="I264" s="15"/>
+      <c r="H264" s="104" t="s">
+        <v>762</v>
+      </c>
+      <c r="I264" s="28"/>
       <c r="J264" s="15"/>
       <c r="K264" s="27" t="s">
         <v>337</v>
       </c>
-      <c r="L264" s="15"/>
+      <c r="L264" s="16"/>
       <c r="M264" s="27"/>
       <c r="N264" s="27"/>
       <c r="O264" s="27"/>
@@ -18741,41 +18741,40 @@
         <v>776</v>
       </c>
     </row>
-    <row r="265" spans="1:24" s="54" customFormat="1" ht="16">
+    <row r="265" spans="1:24" s="54" customFormat="1" ht="15">
       <c r="A265" s="59"/>
-      <c r="B265" s="110" t="s">
-        <v>937</v>
-      </c>
-      <c r="C265" s="15"/>
-      <c r="D265" s="83" t="s">
-        <v>939</v>
-      </c>
-      <c r="E265" s="83" t="s">
-        <v>933</v>
+      <c r="B265" s="49" t="s">
+        <v>151</v>
+      </c>
+      <c r="C265" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="D265" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="E265" s="15" t="s">
+        <v>133</v>
       </c>
       <c r="F265" s="15" t="s">
         <v>197</v>
       </c>
       <c r="G265" s="15"/>
-      <c r="H265" s="104" t="s">
-        <v>762</v>
-      </c>
-      <c r="I265" s="28" t="s">
-        <v>715</v>
-      </c>
+      <c r="H265" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="I265" s="15"/>
       <c r="J265" s="15"/>
       <c r="K265" s="27" t="s">
         <v>337</v>
       </c>
       <c r="L265" s="15"/>
-      <c r="M265" s="47" t="s">
-        <v>374</v>
-      </c>
+      <c r="M265" s="27"/>
       <c r="N265" s="27"/>
-      <c r="O265" s="89">
-        <v>2000000130</v>
-      </c>
-      <c r="P265" s="28"/>
+      <c r="O265" s="27"/>
+      <c r="P265" s="28" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
       <c r="Q265" s="27"/>
       <c r="R265" s="27"/>
       <c r="S265" s="27"/>
@@ -18784,20 +18783,20 @@
       <c r="V265" s="27"/>
       <c r="W265" s="27"/>
       <c r="X265" s="15" t="s">
-        <v>943</v>
+        <v>776</v>
       </c>
     </row>
     <row r="266" spans="1:24" s="54" customFormat="1" ht="16">
       <c r="A266" s="59"/>
       <c r="B266" s="110" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
       <c r="C266" s="15"/>
       <c r="D266" s="83" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
       <c r="E266" s="83" t="s">
-        <v>934</v>
+        <v>931</v>
       </c>
       <c r="F266" s="15" t="s">
         <v>197</v>
@@ -18819,7 +18818,7 @@
       </c>
       <c r="N266" s="27"/>
       <c r="O266" s="89">
-        <v>2000000131</v>
+        <v>2000000130</v>
       </c>
       <c r="P266" s="28"/>
       <c r="Q266" s="27"/>
@@ -18830,18 +18829,20 @@
       <c r="V266" s="27"/>
       <c r="W266" s="27"/>
       <c r="X266" s="15" t="s">
-        <v>944</v>
+        <v>941</v>
       </c>
     </row>
     <row r="267" spans="1:24" s="54" customFormat="1" ht="16">
       <c r="A267" s="59"/>
-      <c r="B267" s="49"/>
+      <c r="B267" s="110" t="s">
+        <v>936</v>
+      </c>
       <c r="C267" s="15"/>
       <c r="D267" s="83" t="s">
-        <v>941</v>
+        <v>938</v>
       </c>
       <c r="E267" s="83" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="F267" s="15" t="s">
         <v>197</v>
@@ -18863,7 +18864,7 @@
       </c>
       <c r="N267" s="27"/>
       <c r="O267" s="89">
-        <v>2000000132</v>
+        <v>2000000131</v>
       </c>
       <c r="P267" s="28"/>
       <c r="Q267" s="27"/>
@@ -18874,7 +18875,7 @@
       <c r="V267" s="27"/>
       <c r="W267" s="27"/>
       <c r="X267" s="15" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
     </row>
     <row r="268" spans="1:24" s="54" customFormat="1" ht="16">
@@ -18882,10 +18883,10 @@
       <c r="B268" s="49"/>
       <c r="C268" s="15"/>
       <c r="D268" s="83" t="s">
-        <v>942</v>
+        <v>939</v>
       </c>
       <c r="E268" s="83" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
       <c r="F268" s="15" t="s">
         <v>197</v>
@@ -18907,7 +18908,7 @@
       </c>
       <c r="N268" s="27"/>
       <c r="O268" s="89">
-        <v>2000000133</v>
+        <v>2000000132</v>
       </c>
       <c r="P268" s="28"/>
       <c r="Q268" s="27"/>
@@ -18918,70 +18919,64 @@
       <c r="V268" s="27"/>
       <c r="W268" s="27"/>
       <c r="X268" s="15" t="s">
-        <v>944</v>
-      </c>
-    </row>
-    <row r="269" spans="1:24" s="54" customFormat="1" ht="44" customHeight="1">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="269" spans="1:24" s="54" customFormat="1" ht="16">
       <c r="A269" s="59"/>
-      <c r="B269" s="110" t="s">
-        <v>790</v>
-      </c>
-      <c r="C269" s="27"/>
-      <c r="D269" s="27" t="s">
-        <v>810</v>
-      </c>
-      <c r="E269" s="45" t="s">
-        <v>791</v>
-      </c>
-      <c r="F269" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="G269" s="15" t="s">
-        <v>792</v>
-      </c>
+      <c r="B269" s="49"/>
+      <c r="C269" s="15"/>
+      <c r="D269" s="83" t="s">
+        <v>940</v>
+      </c>
+      <c r="E269" s="83" t="s">
+        <v>934</v>
+      </c>
+      <c r="F269" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="G269" s="15"/>
       <c r="H269" s="104" t="s">
-        <v>666</v>
+        <v>762</v>
       </c>
       <c r="I269" s="28" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="J269" s="15"/>
       <c r="K269" s="27" t="s">
         <v>337</v>
       </c>
-      <c r="L269" s="16"/>
-      <c r="M269" s="27" t="s">
-        <v>367</v>
+      <c r="L269" s="15"/>
+      <c r="M269" s="47" t="s">
+        <v>374</v>
       </c>
       <c r="N269" s="27"/>
-      <c r="O269" s="27">
-        <v>2000000107</v>
+      <c r="O269" s="89">
+        <v>2000000133</v>
       </c>
       <c r="P269" s="28"/>
       <c r="Q269" s="27"/>
       <c r="R269" s="27"/>
       <c r="S269" s="27"/>
-      <c r="T269" s="15" t="s">
-        <v>667</v>
-      </c>
-      <c r="U269" s="15" t="s">
-        <v>673</v>
-      </c>
+      <c r="T269" s="27"/>
+      <c r="U269" s="27"/>
       <c r="V269" s="27"/>
       <c r="W269" s="27"/>
       <c r="X269" s="15" t="s">
-        <v>774</v>
+        <v>942</v>
       </c>
     </row>
     <row r="270" spans="1:24" s="54" customFormat="1" ht="44" customHeight="1">
       <c r="A270" s="59"/>
-      <c r="B270" s="49"/>
+      <c r="B270" s="110" t="s">
+        <v>790</v>
+      </c>
       <c r="C270" s="27"/>
       <c r="D270" s="27" t="s">
-        <v>795</v>
+        <v>810</v>
       </c>
       <c r="E270" s="45" t="s">
-        <v>800</v>
+        <v>791</v>
       </c>
       <c r="F270" s="27" t="s">
         <v>55</v>
@@ -19005,7 +19000,7 @@
       </c>
       <c r="N270" s="27"/>
       <c r="O270" s="27">
-        <v>2000000108</v>
+        <v>2000000107</v>
       </c>
       <c r="P270" s="28"/>
       <c r="Q270" s="27"/>
@@ -19028,10 +19023,10 @@
       <c r="B271" s="49"/>
       <c r="C271" s="27"/>
       <c r="D271" s="27" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="E271" s="45" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="F271" s="27" t="s">
         <v>55</v>
@@ -19055,7 +19050,7 @@
       </c>
       <c r="N271" s="27"/>
       <c r="O271" s="27">
-        <v>2000000109</v>
+        <v>2000000108</v>
       </c>
       <c r="P271" s="28"/>
       <c r="Q271" s="27"/>
@@ -19070,7 +19065,7 @@
       <c r="V271" s="27"/>
       <c r="W271" s="27"/>
       <c r="X271" s="15" t="s">
-        <v>780</v>
+        <v>774</v>
       </c>
     </row>
     <row r="272" spans="1:24" s="54" customFormat="1" ht="44" customHeight="1">
@@ -19078,10 +19073,10 @@
       <c r="B272" s="49"/>
       <c r="C272" s="27"/>
       <c r="D272" s="27" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="E272" s="45" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="F272" s="27" t="s">
         <v>55</v>
@@ -19105,7 +19100,7 @@
       </c>
       <c r="N272" s="27"/>
       <c r="O272" s="27">
-        <v>2000000110</v>
+        <v>2000000109</v>
       </c>
       <c r="P272" s="28"/>
       <c r="Q272" s="27"/>
@@ -19120,7 +19115,7 @@
       <c r="V272" s="27"/>
       <c r="W272" s="27"/>
       <c r="X272" s="15" t="s">
-        <v>775</v>
+        <v>780</v>
       </c>
     </row>
     <row r="273" spans="1:24" s="54" customFormat="1" ht="44" customHeight="1">
@@ -19128,10 +19123,10 @@
       <c r="B273" s="49"/>
       <c r="C273" s="27"/>
       <c r="D273" s="27" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="E273" s="45" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="F273" s="27" t="s">
         <v>55</v>
@@ -19155,7 +19150,7 @@
       </c>
       <c r="N273" s="27"/>
       <c r="O273" s="27">
-        <v>2000000111</v>
+        <v>2000000110</v>
       </c>
       <c r="P273" s="28"/>
       <c r="Q273" s="27"/>
@@ -19170,30 +19165,30 @@
       <c r="V273" s="27"/>
       <c r="W273" s="27"/>
       <c r="X273" s="15" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="274" spans="1:24" s="54" customFormat="1" ht="44" customHeight="1">
       <c r="A274" s="59"/>
-      <c r="B274" s="110" t="s">
-        <v>803</v>
-      </c>
+      <c r="B274" s="49"/>
       <c r="C274" s="27"/>
-      <c r="D274" s="54" t="s">
-        <v>809</v>
+      <c r="D274" s="27" t="s">
+        <v>796</v>
       </c>
       <c r="E274" s="45" t="s">
-        <v>808</v>
+        <v>797</v>
       </c>
       <c r="F274" s="27" t="s">
-        <v>197</v>
-      </c>
-      <c r="G274" s="15"/>
+        <v>55</v>
+      </c>
+      <c r="G274" s="15" t="s">
+        <v>792</v>
+      </c>
       <c r="H274" s="104" t="s">
-        <v>760</v>
+        <v>666</v>
       </c>
       <c r="I274" s="28" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="J274" s="15"/>
       <c r="K274" s="27" t="s">
@@ -19201,33 +19196,39 @@
       </c>
       <c r="L274" s="16"/>
       <c r="M274" s="27" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="N274" s="27"/>
       <c r="O274" s="27">
-        <v>2000000112</v>
+        <v>2000000111</v>
       </c>
       <c r="P274" s="28"/>
       <c r="Q274" s="27"/>
       <c r="R274" s="27"/>
       <c r="S274" s="27"/>
-      <c r="T274" s="15"/>
-      <c r="U274" s="15"/>
+      <c r="T274" s="15" t="s">
+        <v>667</v>
+      </c>
+      <c r="U274" s="15" t="s">
+        <v>673</v>
+      </c>
       <c r="V274" s="27"/>
       <c r="W274" s="27"/>
       <c r="X274" s="15" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
     </row>
     <row r="275" spans="1:24" s="54" customFormat="1" ht="44" customHeight="1">
       <c r="A275" s="59"/>
-      <c r="B275" s="49"/>
+      <c r="B275" s="110" t="s">
+        <v>803</v>
+      </c>
       <c r="C275" s="27"/>
-      <c r="D275" s="27" t="s">
-        <v>804</v>
+      <c r="D275" s="54" t="s">
+        <v>809</v>
       </c>
       <c r="E275" s="45" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="F275" s="27" t="s">
         <v>197</v>
@@ -19249,7 +19250,7 @@
       </c>
       <c r="N275" s="27"/>
       <c r="O275" s="27">
-        <v>2000000113</v>
+        <v>2000000112</v>
       </c>
       <c r="P275" s="28"/>
       <c r="Q275" s="27"/>
@@ -19260,7 +19261,7 @@
       <c r="V275" s="27"/>
       <c r="W275" s="27"/>
       <c r="X275" s="15" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="276" spans="1:24" s="54" customFormat="1" ht="44" customHeight="1">
@@ -19268,10 +19269,10 @@
       <c r="B276" s="49"/>
       <c r="C276" s="27"/>
       <c r="D276" s="27" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E276" s="45" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="F276" s="27" t="s">
         <v>197</v>
@@ -19293,7 +19294,7 @@
       </c>
       <c r="N276" s="27"/>
       <c r="O276" s="27">
-        <v>2000000114</v>
+        <v>2000000113</v>
       </c>
       <c r="P276" s="28"/>
       <c r="Q276" s="27"/>
@@ -19304,7 +19305,7 @@
       <c r="V276" s="27"/>
       <c r="W276" s="27"/>
       <c r="X276" s="15" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="277" spans="1:24" s="54" customFormat="1" ht="44" customHeight="1">
@@ -19312,10 +19313,10 @@
       <c r="B277" s="49"/>
       <c r="C277" s="27"/>
       <c r="D277" s="27" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E277" s="45" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="F277" s="27" t="s">
         <v>197</v>
@@ -19337,7 +19338,7 @@
       </c>
       <c r="N277" s="27"/>
       <c r="O277" s="27">
-        <v>2000000115</v>
+        <v>2000000114</v>
       </c>
       <c r="P277" s="28"/>
       <c r="Q277" s="27"/>
@@ -19348,7 +19349,7 @@
       <c r="V277" s="27"/>
       <c r="W277" s="27"/>
       <c r="X277" s="15" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
     </row>
     <row r="278" spans="1:24" s="54" customFormat="1" ht="44" customHeight="1">
@@ -19356,10 +19357,10 @@
       <c r="B278" s="49"/>
       <c r="C278" s="27"/>
       <c r="D278" s="27" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E278" s="45" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="F278" s="27" t="s">
         <v>197</v>
@@ -19381,7 +19382,7 @@
       </c>
       <c r="N278" s="27"/>
       <c r="O278" s="27">
-        <v>2000000116</v>
+        <v>2000000115</v>
       </c>
       <c r="P278" s="28"/>
       <c r="Q278" s="27"/>
@@ -19392,95 +19393,90 @@
       <c r="V278" s="27"/>
       <c r="W278" s="27"/>
       <c r="X278" s="15" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="279" spans="1:24" s="54" customFormat="1" ht="44" customHeight="1">
+      <c r="A279" s="59"/>
+      <c r="B279" s="49"/>
+      <c r="C279" s="27"/>
+      <c r="D279" s="27" t="s">
+        <v>807</v>
+      </c>
+      <c r="E279" s="45" t="s">
+        <v>814</v>
+      </c>
+      <c r="F279" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="G279" s="15"/>
+      <c r="H279" s="104" t="s">
+        <v>760</v>
+      </c>
+      <c r="I279" s="28" t="s">
+        <v>715</v>
+      </c>
+      <c r="J279" s="15"/>
+      <c r="K279" s="27" t="s">
+        <v>337</v>
+      </c>
+      <c r="L279" s="16"/>
+      <c r="M279" s="27" t="s">
+        <v>374</v>
+      </c>
+      <c r="N279" s="27"/>
+      <c r="O279" s="27">
+        <v>2000000116</v>
+      </c>
+      <c r="P279" s="28"/>
+      <c r="Q279" s="27"/>
+      <c r="R279" s="27"/>
+      <c r="S279" s="27"/>
+      <c r="T279" s="15"/>
+      <c r="U279" s="15"/>
+      <c r="V279" s="27"/>
+      <c r="W279" s="27"/>
+      <c r="X279" s="15" t="s">
         <v>780</v>
       </c>
     </row>
-    <row r="279" spans="1:24" s="54" customFormat="1" ht="15">
-      <c r="A279" s="75" t="s">
+    <row r="280" spans="1:24" s="54" customFormat="1" ht="15">
+      <c r="A280" s="75" t="s">
         <v>271</v>
       </c>
-      <c r="B279" s="48"/>
-      <c r="C279" s="6"/>
-      <c r="D279" s="6"/>
-      <c r="E279" s="7"/>
-      <c r="F279" s="6"/>
-      <c r="G279" s="6"/>
-      <c r="H279" s="30"/>
-      <c r="I279" s="30"/>
-      <c r="J279" s="6"/>
-      <c r="K279" s="53"/>
-      <c r="L279" s="7"/>
-      <c r="M279" s="53"/>
-      <c r="N279" s="53"/>
-      <c r="O279" s="53"/>
-      <c r="P279" s="53"/>
-      <c r="Q279" s="53"/>
-      <c r="R279" s="53"/>
-      <c r="S279" s="53"/>
-      <c r="T279" s="53"/>
-      <c r="U279" s="53"/>
-      <c r="V279" s="53"/>
-      <c r="W279" s="53"/>
-      <c r="X279" s="53"/>
-    </row>
-    <row r="280" spans="1:24" s="54" customFormat="1" ht="15">
-      <c r="A280" s="59"/>
-      <c r="B280" s="49"/>
-      <c r="C280" s="15"/>
-      <c r="D280" s="79" t="s">
-        <v>698</v>
-      </c>
-      <c r="E280" s="15" t="s">
-        <v>283</v>
-      </c>
-      <c r="F280" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="G280" s="15"/>
-      <c r="H280" s="104" t="s">
-        <v>762</v>
-      </c>
-      <c r="I280" s="28" t="s">
-        <v>715</v>
-      </c>
-      <c r="J280" s="15"/>
-      <c r="K280" s="27" t="s">
-        <v>337</v>
-      </c>
-      <c r="L280" s="24"/>
-      <c r="M280" s="27" t="s">
-        <v>374</v>
-      </c>
-      <c r="N280" s="27" t="s">
-        <v>368</v>
-      </c>
-      <c r="O280" s="27">
-        <v>44807681</v>
-      </c>
-      <c r="P280" s="28" t="str">
-        <f t="shared" ref="P280:P293" si="22">IF(N280&lt;&gt;"",HYPERLINK(CONCATENATE("https:;;athena.ohdsi.org;search-terms;terms;",O280), CONCATENATE("Athena-",O280)),"")</f>
-        <v>Athena-44807681</v>
-      </c>
-      <c r="Q280" s="27"/>
-      <c r="R280" s="27"/>
-      <c r="S280" s="27"/>
-      <c r="T280" s="27"/>
-      <c r="U280" s="27"/>
-      <c r="V280" s="27"/>
-      <c r="W280" s="27"/>
-      <c r="X280" s="27" t="s">
-        <v>771</v>
-      </c>
-    </row>
-    <row r="281" spans="1:24" s="54" customFormat="1" ht="16">
+      <c r="B280" s="48"/>
+      <c r="C280" s="6"/>
+      <c r="D280" s="6"/>
+      <c r="E280" s="7"/>
+      <c r="F280" s="6"/>
+      <c r="G280" s="6"/>
+      <c r="H280" s="30"/>
+      <c r="I280" s="30"/>
+      <c r="J280" s="6"/>
+      <c r="K280" s="53"/>
+      <c r="L280" s="7"/>
+      <c r="M280" s="53"/>
+      <c r="N280" s="53"/>
+      <c r="O280" s="53"/>
+      <c r="P280" s="53"/>
+      <c r="Q280" s="53"/>
+      <c r="R280" s="53"/>
+      <c r="S280" s="53"/>
+      <c r="T280" s="53"/>
+      <c r="U280" s="53"/>
+      <c r="V280" s="53"/>
+      <c r="W280" s="53"/>
+      <c r="X280" s="53"/>
+    </row>
+    <row r="281" spans="1:24" s="54" customFormat="1" ht="15">
       <c r="A281" s="59"/>
       <c r="B281" s="49"/>
-      <c r="C281" s="16"/>
-      <c r="D281" s="80" t="s">
-        <v>699</v>
-      </c>
-      <c r="E281" s="16" t="s">
-        <v>284</v>
+      <c r="C281" s="15"/>
+      <c r="D281" s="79" t="s">
+        <v>698</v>
+      </c>
+      <c r="E281" s="15" t="s">
+        <v>283</v>
       </c>
       <c r="F281" s="15" t="s">
         <v>197</v>
@@ -19496,27 +19492,23 @@
       <c r="K281" s="27" t="s">
         <v>337</v>
       </c>
-      <c r="L281" s="16"/>
+      <c r="L281" s="24"/>
       <c r="M281" s="27" t="s">
         <v>374</v>
       </c>
-      <c r="N281" s="27"/>
+      <c r="N281" s="27" t="s">
+        <v>368</v>
+      </c>
       <c r="O281" s="27">
-        <v>2000000093</v>
+        <v>44807681</v>
       </c>
       <c r="P281" s="28" t="str">
-        <f>IF(N281&lt;&gt;"",HYPERLINK(CONCATENATE("https:;;athena.ohdsi.org;search-terms;terms;",O281), CONCATENATE("Athena-",O281)),"")</f>
-        <v/>
-      </c>
-      <c r="Q281" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="R281" s="27">
-        <v>8845</v>
-      </c>
-      <c r="S281" s="27" t="s">
-        <v>376</v>
-      </c>
+        <f t="shared" ref="P281:P294" si="22">IF(N281&lt;&gt;"",HYPERLINK(CONCATENATE("https:;;athena.ohdsi.org;search-terms;terms;",O281), CONCATENATE("Athena-",O281)),"")</f>
+        <v>Athena-44807681</v>
+      </c>
+      <c r="Q281" s="27"/>
+      <c r="R281" s="27"/>
+      <c r="S281" s="27"/>
       <c r="T281" s="27"/>
       <c r="U281" s="27"/>
       <c r="V281" s="27"/>
@@ -19530,15 +19522,15 @@
       <c r="B282" s="49"/>
       <c r="C282" s="16"/>
       <c r="D282" s="80" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="E282" s="16" t="s">
-        <v>585</v>
+        <v>284</v>
       </c>
       <c r="F282" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="G282" s="16"/>
+      <c r="G282" s="15"/>
       <c r="H282" s="104" t="s">
         <v>762</v>
       </c>
@@ -19555,7 +19547,7 @@
       </c>
       <c r="N282" s="27"/>
       <c r="O282" s="27">
-        <v>2000000094</v>
+        <v>2000000093</v>
       </c>
       <c r="P282" s="28" t="str">
         <f>IF(N282&lt;&gt;"",HYPERLINK(CONCATENATE("https:;;athena.ohdsi.org;search-terms;terms;",O282), CONCATENATE("Athena-",O282)),"")</f>
@@ -19583,10 +19575,10 @@
       <c r="B283" s="49"/>
       <c r="C283" s="16"/>
       <c r="D283" s="80" t="s">
-        <v>772</v>
+        <v>700</v>
       </c>
       <c r="E283" s="16" t="s">
-        <v>773</v>
+        <v>585</v>
       </c>
       <c r="F283" s="15" t="s">
         <v>197</v>
@@ -19608,15 +19600,21 @@
       </c>
       <c r="N283" s="27"/>
       <c r="O283" s="27">
-        <v>2000000105</v>
+        <v>2000000094</v>
       </c>
       <c r="P283" s="28" t="str">
         <f>IF(N283&lt;&gt;"",HYPERLINK(CONCATENATE("https:;;athena.ohdsi.org;search-terms;terms;",O283), CONCATENATE("Athena-",O283)),"")</f>
         <v/>
       </c>
-      <c r="Q283" s="27"/>
-      <c r="R283" s="27"/>
-      <c r="S283" s="27"/>
+      <c r="Q283" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="R283" s="27">
+        <v>8845</v>
+      </c>
+      <c r="S283" s="27" t="s">
+        <v>376</v>
+      </c>
       <c r="T283" s="27"/>
       <c r="U283" s="27"/>
       <c r="V283" s="27"/>
@@ -19630,15 +19628,15 @@
       <c r="B284" s="49"/>
       <c r="C284" s="16"/>
       <c r="D284" s="80" t="s">
-        <v>274</v>
+        <v>772</v>
       </c>
       <c r="E284" s="16" t="s">
-        <v>285</v>
+        <v>773</v>
       </c>
       <c r="F284" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="G284" s="15"/>
+      <c r="G284" s="16"/>
       <c r="H284" s="104" t="s">
         <v>762</v>
       </c>
@@ -19655,10 +19653,10 @@
       </c>
       <c r="N284" s="27"/>
       <c r="O284" s="27">
-        <v>2000000095</v>
+        <v>2000000105</v>
       </c>
       <c r="P284" s="28" t="str">
-        <f t="shared" si="22"/>
+        <f>IF(N284&lt;&gt;"",HYPERLINK(CONCATENATE("https:;;athena.ohdsi.org;search-terms;terms;",O284), CONCATENATE("Athena-",O284)),"")</f>
         <v/>
       </c>
       <c r="Q284" s="27"/>
@@ -19675,12 +19673,12 @@
     <row r="285" spans="1:24" s="54" customFormat="1" ht="16">
       <c r="A285" s="59"/>
       <c r="B285" s="49"/>
-      <c r="C285" s="15"/>
-      <c r="D285" s="79" t="s">
-        <v>275</v>
-      </c>
-      <c r="E285" s="45" t="s">
-        <v>286</v>
+      <c r="C285" s="16"/>
+      <c r="D285" s="80" t="s">
+        <v>274</v>
+      </c>
+      <c r="E285" s="16" t="s">
+        <v>285</v>
       </c>
       <c r="F285" s="15" t="s">
         <v>197</v>
@@ -19701,8 +19699,8 @@
         <v>374</v>
       </c>
       <c r="N285" s="27"/>
-      <c r="O285" s="79">
-        <v>2000000096</v>
+      <c r="O285" s="27">
+        <v>2000000095</v>
       </c>
       <c r="P285" s="28" t="str">
         <f t="shared" si="22"/>
@@ -19724,10 +19722,10 @@
       <c r="B286" s="49"/>
       <c r="C286" s="15"/>
       <c r="D286" s="79" t="s">
-        <v>701</v>
-      </c>
-      <c r="E286" s="11" t="s">
-        <v>288</v>
+        <v>275</v>
+      </c>
+      <c r="E286" s="45" t="s">
+        <v>286</v>
       </c>
       <c r="F286" s="15" t="s">
         <v>197</v>
@@ -19748,8 +19746,8 @@
         <v>374</v>
       </c>
       <c r="N286" s="27"/>
-      <c r="O286" s="27">
-        <v>2000000097</v>
+      <c r="O286" s="79">
+        <v>2000000096</v>
       </c>
       <c r="P286" s="28" t="str">
         <f t="shared" si="22"/>
@@ -19769,17 +19767,17 @@
     <row r="287" spans="1:24" s="54" customFormat="1" ht="16">
       <c r="A287" s="59"/>
       <c r="B287" s="49"/>
-      <c r="C287" s="16"/>
-      <c r="D287" s="80" t="s">
-        <v>276</v>
-      </c>
-      <c r="E287" s="16" t="s">
-        <v>289</v>
+      <c r="C287" s="15"/>
+      <c r="D287" s="79" t="s">
+        <v>701</v>
+      </c>
+      <c r="E287" s="11" t="s">
+        <v>288</v>
       </c>
       <c r="F287" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="G287" s="16"/>
+      <c r="G287" s="15"/>
       <c r="H287" s="104" t="s">
         <v>762</v>
       </c>
@@ -19794,15 +19792,13 @@
       <c r="M287" s="27" t="s">
         <v>374</v>
       </c>
-      <c r="N287" s="27" t="s">
-        <v>368</v>
-      </c>
+      <c r="N287" s="27"/>
       <c r="O287" s="27">
-        <v>46284972</v>
+        <v>2000000097</v>
       </c>
       <c r="P287" s="28" t="str">
         <f t="shared" si="22"/>
-        <v>Athena-46284972</v>
+        <v/>
       </c>
       <c r="Q287" s="27"/>
       <c r="R287" s="27"/>
@@ -19820,15 +19816,15 @@
       <c r="B288" s="49"/>
       <c r="C288" s="16"/>
       <c r="D288" s="80" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E288" s="16" t="s">
-        <v>378</v>
+        <v>289</v>
       </c>
       <c r="F288" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="G288" s="15"/>
+      <c r="G288" s="16"/>
       <c r="H288" s="104" t="s">
         <v>762</v>
       </c>
@@ -19843,13 +19839,15 @@
       <c r="M288" s="27" t="s">
         <v>374</v>
       </c>
-      <c r="N288" s="27"/>
+      <c r="N288" s="27" t="s">
+        <v>368</v>
+      </c>
       <c r="O288" s="27">
-        <v>2000000098</v>
+        <v>46284972</v>
       </c>
       <c r="P288" s="28" t="str">
         <f t="shared" si="22"/>
-        <v/>
+        <v>Athena-46284972</v>
       </c>
       <c r="Q288" s="27"/>
       <c r="R288" s="27"/>
@@ -19865,12 +19863,12 @@
     <row r="289" spans="1:25" s="54" customFormat="1" ht="16">
       <c r="A289" s="59"/>
       <c r="B289" s="49"/>
-      <c r="C289" s="15"/>
-      <c r="D289" s="79" t="s">
-        <v>278</v>
-      </c>
-      <c r="E289" s="45" t="s">
-        <v>377</v>
+      <c r="C289" s="16"/>
+      <c r="D289" s="80" t="s">
+        <v>277</v>
+      </c>
+      <c r="E289" s="16" t="s">
+        <v>378</v>
       </c>
       <c r="F289" s="15" t="s">
         <v>197</v>
@@ -19892,7 +19890,7 @@
       </c>
       <c r="N289" s="27"/>
       <c r="O289" s="27">
-        <v>2000000099</v>
+        <v>2000000098</v>
       </c>
       <c r="P289" s="28" t="str">
         <f t="shared" si="22"/>
@@ -19911,25 +19909,25 @@
     </row>
     <row r="290" spans="1:25" s="54" customFormat="1" ht="16">
       <c r="A290" s="59"/>
-      <c r="B290" s="16"/>
-      <c r="C290" s="16"/>
-      <c r="D290" s="80" t="s">
-        <v>279</v>
-      </c>
-      <c r="E290" s="16" t="s">
-        <v>290</v>
+      <c r="B290" s="49"/>
+      <c r="C290" s="15"/>
+      <c r="D290" s="79" t="s">
+        <v>278</v>
+      </c>
+      <c r="E290" s="45" t="s">
+        <v>377</v>
       </c>
       <c r="F290" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="G290" s="16"/>
+      <c r="G290" s="15"/>
       <c r="H290" s="104" t="s">
         <v>762</v>
       </c>
       <c r="I290" s="28" t="s">
         <v>715</v>
       </c>
-      <c r="J290" s="16"/>
+      <c r="J290" s="15"/>
       <c r="K290" s="27" t="s">
         <v>337</v>
       </c>
@@ -19937,15 +19935,13 @@
       <c r="M290" s="27" t="s">
         <v>374</v>
       </c>
-      <c r="N290" s="27" t="s">
-        <v>368</v>
-      </c>
+      <c r="N290" s="27"/>
       <c r="O290" s="27">
-        <v>4332015</v>
+        <v>2000000099</v>
       </c>
       <c r="P290" s="28" t="str">
         <f t="shared" si="22"/>
-        <v>Athena-4332015</v>
+        <v/>
       </c>
       <c r="Q290" s="27"/>
       <c r="R290" s="27"/>
@@ -19963,10 +19959,10 @@
       <c r="B291" s="16"/>
       <c r="C291" s="16"/>
       <c r="D291" s="80" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E291" s="16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F291" s="15" t="s">
         <v>197</v>
@@ -19990,11 +19986,11 @@
         <v>368</v>
       </c>
       <c r="O291" s="27">
-        <v>4166200</v>
+        <v>4332015</v>
       </c>
       <c r="P291" s="28" t="str">
         <f t="shared" si="22"/>
-        <v>Athena-4166200</v>
+        <v>Athena-4332015</v>
       </c>
       <c r="Q291" s="27"/>
       <c r="R291" s="27"/>
@@ -20012,10 +20008,10 @@
       <c r="B292" s="16"/>
       <c r="C292" s="16"/>
       <c r="D292" s="80" t="s">
-        <v>702</v>
+        <v>280</v>
       </c>
       <c r="E292" s="16" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F292" s="15" t="s">
         <v>197</v>
@@ -20039,11 +20035,11 @@
         <v>368</v>
       </c>
       <c r="O292" s="27">
-        <v>4282774</v>
+        <v>4166200</v>
       </c>
       <c r="P292" s="28" t="str">
         <f t="shared" si="22"/>
-        <v>Athena-4282774</v>
+        <v>Athena-4166200</v>
       </c>
       <c r="Q292" s="27"/>
       <c r="R292" s="27"/>
@@ -20061,10 +20057,10 @@
       <c r="B293" s="16"/>
       <c r="C293" s="16"/>
       <c r="D293" s="80" t="s">
-        <v>282</v>
+        <v>702</v>
       </c>
       <c r="E293" s="16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F293" s="15" t="s">
         <v>197</v>
@@ -20084,13 +20080,15 @@
       <c r="M293" s="27" t="s">
         <v>374</v>
       </c>
-      <c r="N293" s="27"/>
+      <c r="N293" s="27" t="s">
+        <v>368</v>
+      </c>
       <c r="O293" s="27">
-        <v>2000000076</v>
+        <v>4282774</v>
       </c>
       <c r="P293" s="28" t="str">
         <f t="shared" si="22"/>
-        <v/>
+        <v>Athena-4282774</v>
       </c>
       <c r="Q293" s="27"/>
       <c r="R293" s="27"/>
@@ -20108,10 +20106,10 @@
       <c r="B294" s="16"/>
       <c r="C294" s="16"/>
       <c r="D294" s="80" t="s">
-        <v>781</v>
+        <v>282</v>
       </c>
       <c r="E294" s="16" t="s">
-        <v>782</v>
+        <v>293</v>
       </c>
       <c r="F294" s="15" t="s">
         <v>197</v>
@@ -20131,19 +20129,15 @@
       <c r="M294" s="27" t="s">
         <v>374</v>
       </c>
-      <c r="N294" s="27" t="s">
-        <v>368</v>
-      </c>
+      <c r="N294" s="27"/>
       <c r="O294" s="27">
-        <v>4056962</v>
+        <v>2000000076</v>
       </c>
       <c r="P294" s="28" t="str">
-        <f t="shared" ref="P294" si="23">IF(N294&lt;&gt;"",HYPERLINK(CONCATENATE("https:;;athena.ohdsi.org;search-terms;terms;",O294), CONCATENATE("Athena-",O294)),"")</f>
-        <v>Athena-4056962</v>
-      </c>
-      <c r="Q294" s="27" t="s">
-        <v>783</v>
-      </c>
+        <f t="shared" si="22"/>
+        <v/>
+      </c>
+      <c r="Q294" s="27"/>
       <c r="R294" s="27"/>
       <c r="S294" s="27"/>
       <c r="T294" s="27"/>
@@ -20153,29 +20147,60 @@
       <c r="X294" s="27" t="s">
         <v>771</v>
       </c>
-      <c r="Y294" s="54" t="s">
+    </row>
+    <row r="295" spans="1:25" s="54" customFormat="1" ht="16">
+      <c r="A295" s="59"/>
+      <c r="B295" s="16"/>
+      <c r="C295" s="16"/>
+      <c r="D295" s="80" t="s">
+        <v>781</v>
+      </c>
+      <c r="E295" s="16" t="s">
+        <v>782</v>
+      </c>
+      <c r="F295" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="G295" s="16"/>
+      <c r="H295" s="104" t="s">
+        <v>762</v>
+      </c>
+      <c r="I295" s="28" t="s">
+        <v>715</v>
+      </c>
+      <c r="J295" s="16"/>
+      <c r="K295" s="27" t="s">
+        <v>337</v>
+      </c>
+      <c r="L295" s="16"/>
+      <c r="M295" s="27" t="s">
+        <v>374</v>
+      </c>
+      <c r="N295" s="27" t="s">
+        <v>368</v>
+      </c>
+      <c r="O295" s="27">
+        <v>4056962</v>
+      </c>
+      <c r="P295" s="28" t="str">
+        <f t="shared" ref="P295" si="23">IF(N295&lt;&gt;"",HYPERLINK(CONCATENATE("https:;;athena.ohdsi.org;search-terms;terms;",O295), CONCATENATE("Athena-",O295)),"")</f>
+        <v>Athena-4056962</v>
+      </c>
+      <c r="Q295" s="27" t="s">
+        <v>783</v>
+      </c>
+      <c r="R295" s="27"/>
+      <c r="S295" s="27"/>
+      <c r="T295" s="27"/>
+      <c r="U295" s="27"/>
+      <c r="V295" s="27"/>
+      <c r="W295" s="27"/>
+      <c r="X295" s="27" t="s">
+        <v>771</v>
+      </c>
+      <c r="Y295" s="54" t="s">
         <v>785</v>
       </c>
-    </row>
-    <row r="295" spans="1:25">
-      <c r="G295" s="23"/>
-      <c r="H295" s="34"/>
-      <c r="I295" s="34"/>
-      <c r="J295" s="23"/>
-      <c r="K295" s="40"/>
-      <c r="L295" s="23"/>
-      <c r="M295" s="40"/>
-      <c r="N295" s="40"/>
-      <c r="O295" s="40"/>
-      <c r="P295" s="40"/>
-      <c r="Q295" s="40"/>
-      <c r="R295" s="40"/>
-      <c r="S295" s="40"/>
-      <c r="T295" s="40"/>
-      <c r="U295" s="40"/>
-      <c r="V295" s="40"/>
-      <c r="W295" s="40"/>
-      <c r="X295" s="40"/>
     </row>
     <row r="296" spans="1:25">
       <c r="G296" s="23"/>
@@ -20539,23 +20564,23 @@
     </row>
     <row r="314" spans="7:24">
       <c r="G314" s="23"/>
-      <c r="H314" s="23"/>
-      <c r="I314" s="23"/>
+      <c r="H314" s="34"/>
+      <c r="I314" s="34"/>
       <c r="J314" s="23"/>
-      <c r="K314" s="23"/>
+      <c r="K314" s="40"/>
       <c r="L314" s="23"/>
-      <c r="M314" s="23"/>
-      <c r="N314" s="23"/>
-      <c r="O314" s="23"/>
-      <c r="P314" s="23"/>
-      <c r="Q314" s="23"/>
-      <c r="R314" s="23"/>
-      <c r="S314" s="23"/>
-      <c r="T314" s="23"/>
-      <c r="U314" s="23"/>
-      <c r="V314" s="23"/>
-      <c r="W314" s="23"/>
-      <c r="X314" s="23"/>
+      <c r="M314" s="40"/>
+      <c r="N314" s="40"/>
+      <c r="O314" s="40"/>
+      <c r="P314" s="40"/>
+      <c r="Q314" s="40"/>
+      <c r="R314" s="40"/>
+      <c r="S314" s="40"/>
+      <c r="T314" s="40"/>
+      <c r="U314" s="40"/>
+      <c r="V314" s="40"/>
+      <c r="W314" s="40"/>
+      <c r="X314" s="40"/>
     </row>
     <row r="315" spans="7:24">
       <c r="G315" s="23"/>
@@ -39597,6 +39622,26 @@
       <c r="W1266" s="23"/>
       <c r="X1266" s="23"/>
     </row>
+    <row r="1267" spans="7:24">
+      <c r="G1267" s="23"/>
+      <c r="H1267" s="23"/>
+      <c r="I1267" s="23"/>
+      <c r="J1267" s="23"/>
+      <c r="K1267" s="23"/>
+      <c r="L1267" s="23"/>
+      <c r="M1267" s="23"/>
+      <c r="N1267" s="23"/>
+      <c r="O1267" s="23"/>
+      <c r="P1267" s="23"/>
+      <c r="Q1267" s="23"/>
+      <c r="R1267" s="23"/>
+      <c r="S1267" s="23"/>
+      <c r="T1267" s="23"/>
+      <c r="U1267" s="23"/>
+      <c r="V1267" s="23"/>
+      <c r="W1267" s="23"/>
+      <c r="X1267" s="23"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -39613,7 +39658,7 @@
   <dimension ref="A1:Y30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T24" sqref="T24"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Included brain age and metabo age as variables
</commit_message>
<xml_diff>
--- a/ncdc_mappings/ncdc_minimal_dataset.xlsx
+++ b/ncdc_mappings/ncdc_minimal_dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://maastro-my.sharepoint.com/personal/pedro_mateus_maastro_nl/Documents/Pedro Files/Data Harmonization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="13_ncr:1_{CFD7E28C-48FE-9D4B-9FBD-FF4601B5D85E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BACBD9F7-2791-224F-9B2F-4236BA550120}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="13_ncr:1_{CFD7E28C-48FE-9D4B-9FBD-FF4601B5D85E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4A56392-EDF4-FC4B-8CD7-A7246C80C7C3}"/>
   <bookViews>
-    <workbookView xWindow="2960" yWindow="500" windowWidth="33600" windowHeight="19260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="500" windowWidth="33600" windowHeight="19260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping" sheetId="2" r:id="rId1"/>
@@ -700,7 +700,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4622" uniqueCount="965">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4644" uniqueCount="973">
   <si>
     <t>Main category</t>
   </si>
@@ -3641,6 +3641,30 @@
   </si>
   <si>
     <t>Attention_test_stroop_2_errors</t>
+  </si>
+  <si>
+    <t>Metabolomics</t>
+  </si>
+  <si>
+    <t>Date_metabolomics</t>
+  </si>
+  <si>
+    <t>metabo_age</t>
+  </si>
+  <si>
+    <t>Predicted age based on the metabolomic data</t>
+  </si>
+  <si>
+    <t>MRI</t>
+  </si>
+  <si>
+    <t>brain_age</t>
+  </si>
+  <si>
+    <t>Predicted age based on the MRI data</t>
+  </si>
+  <si>
+    <t>Date_mri</t>
   </si>
 </sst>
 </file>
@@ -3935,7 +3959,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -4163,6 +4187,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
@@ -5954,8 +5985,8 @@
   <dimension ref="A1:Y1272"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="89" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D177" sqref="D177"/>
+      <pane ySplit="1" topLeftCell="A278" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E313" sqref="E313"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="17"/>
@@ -20465,85 +20496,161 @@
         <v>784</v>
       </c>
     </row>
-    <row r="301" spans="1:25">
-      <c r="G301" s="23"/>
-      <c r="H301" s="34"/>
-      <c r="I301" s="34"/>
-      <c r="J301" s="23"/>
-      <c r="K301" s="40"/>
-      <c r="L301" s="23"/>
-      <c r="M301" s="40"/>
-      <c r="N301" s="40"/>
-      <c r="O301" s="40"/>
-      <c r="P301" s="40"/>
-      <c r="Q301" s="40"/>
-      <c r="R301" s="40"/>
-      <c r="S301" s="40"/>
-      <c r="T301" s="40"/>
-      <c r="U301" s="40"/>
-      <c r="V301" s="40"/>
-      <c r="W301" s="40"/>
-      <c r="X301" s="40"/>
+    <row r="301" spans="1:25" s="54" customFormat="1" ht="15">
+      <c r="A301" s="75" t="s">
+        <v>965</v>
+      </c>
+      <c r="B301" s="48"/>
+      <c r="C301" s="6"/>
+      <c r="D301" s="6"/>
+      <c r="E301" s="7"/>
+      <c r="F301" s="6"/>
+      <c r="G301" s="6"/>
+      <c r="H301" s="30"/>
+      <c r="I301" s="30"/>
+      <c r="J301" s="6"/>
+      <c r="K301" s="53"/>
+      <c r="L301" s="7"/>
+      <c r="M301" s="53"/>
+      <c r="N301" s="53"/>
+      <c r="O301" s="53"/>
+      <c r="P301" s="53"/>
+      <c r="Q301" s="53"/>
+      <c r="R301" s="53"/>
+      <c r="S301" s="53"/>
+      <c r="T301" s="53"/>
+      <c r="U301" s="53"/>
+      <c r="V301" s="53"/>
+      <c r="W301" s="53"/>
+      <c r="X301" s="53"/>
     </row>
     <row r="302" spans="1:25">
-      <c r="G302" s="23"/>
-      <c r="H302" s="34"/>
-      <c r="I302" s="34"/>
-      <c r="J302" s="23"/>
-      <c r="K302" s="40"/>
-      <c r="L302" s="23"/>
-      <c r="M302" s="40"/>
-      <c r="N302" s="40"/>
-      <c r="O302" s="40"/>
-      <c r="P302" s="40"/>
-      <c r="Q302" s="40"/>
-      <c r="R302" s="40"/>
-      <c r="S302" s="40"/>
-      <c r="T302" s="40"/>
-      <c r="U302" s="40"/>
-      <c r="V302" s="40"/>
-      <c r="W302" s="40"/>
-      <c r="X302" s="40"/>
-    </row>
-    <row r="303" spans="1:25">
-      <c r="G303" s="23"/>
-      <c r="H303" s="34"/>
-      <c r="I303" s="34"/>
-      <c r="J303" s="23"/>
-      <c r="K303" s="40"/>
-      <c r="L303" s="23"/>
-      <c r="M303" s="40"/>
-      <c r="N303" s="40"/>
-      <c r="O303" s="40"/>
-      <c r="P303" s="40"/>
-      <c r="Q303" s="40"/>
-      <c r="R303" s="40"/>
-      <c r="S303" s="40"/>
-      <c r="T303" s="40"/>
-      <c r="U303" s="40"/>
-      <c r="V303" s="40"/>
-      <c r="W303" s="40"/>
-      <c r="X303" s="40"/>
+      <c r="A302" s="111"/>
+      <c r="B302" s="111"/>
+      <c r="C302" s="112"/>
+      <c r="D302" s="112" t="s">
+        <v>967</v>
+      </c>
+      <c r="E302" s="113" t="s">
+        <v>968</v>
+      </c>
+      <c r="F302" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="G302" s="112"/>
+      <c r="H302" s="104" t="s">
+        <v>761</v>
+      </c>
+      <c r="I302" s="28" t="s">
+        <v>715</v>
+      </c>
+      <c r="J302" s="112"/>
+      <c r="K302" s="27" t="s">
+        <v>337</v>
+      </c>
+      <c r="L302" s="112"/>
+      <c r="M302" s="27" t="s">
+        <v>374</v>
+      </c>
+      <c r="N302" s="114"/>
+      <c r="O302" s="114">
+        <v>2000000143</v>
+      </c>
+      <c r="P302" s="114"/>
+      <c r="Q302" s="28" t="s">
+        <v>369</v>
+      </c>
+      <c r="R302" s="28">
+        <v>9448</v>
+      </c>
+      <c r="S302" s="27" t="s">
+        <v>376</v>
+      </c>
+      <c r="T302" s="114"/>
+      <c r="U302" s="114"/>
+      <c r="V302" s="114"/>
+      <c r="W302" s="114"/>
+      <c r="X302" s="115" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="303" spans="1:25" s="54" customFormat="1" ht="15">
+      <c r="A303" s="75" t="s">
+        <v>969</v>
+      </c>
+      <c r="B303" s="48"/>
+      <c r="C303" s="6"/>
+      <c r="D303" s="6"/>
+      <c r="E303" s="7"/>
+      <c r="F303" s="6"/>
+      <c r="G303" s="6"/>
+      <c r="H303" s="30"/>
+      <c r="I303" s="30"/>
+      <c r="J303" s="6"/>
+      <c r="K303" s="53"/>
+      <c r="L303" s="7"/>
+      <c r="M303" s="53"/>
+      <c r="N303" s="53"/>
+      <c r="O303" s="53"/>
+      <c r="P303" s="53"/>
+      <c r="Q303" s="53"/>
+      <c r="R303" s="53"/>
+      <c r="S303" s="53"/>
+      <c r="T303" s="53"/>
+      <c r="U303" s="53"/>
+      <c r="V303" s="53"/>
+      <c r="W303" s="53"/>
+      <c r="X303" s="53"/>
     </row>
     <row r="304" spans="1:25">
-      <c r="G304" s="23"/>
-      <c r="H304" s="34"/>
-      <c r="I304" s="34"/>
-      <c r="J304" s="23"/>
-      <c r="K304" s="40"/>
-      <c r="L304" s="23"/>
-      <c r="M304" s="40"/>
-      <c r="N304" s="40"/>
-      <c r="O304" s="40"/>
-      <c r="P304" s="40"/>
-      <c r="Q304" s="40"/>
-      <c r="R304" s="40"/>
-      <c r="S304" s="40"/>
-      <c r="T304" s="40"/>
-      <c r="U304" s="40"/>
-      <c r="V304" s="40"/>
-      <c r="W304" s="40"/>
-      <c r="X304" s="40"/>
+      <c r="A304" s="111"/>
+      <c r="B304" s="111"/>
+      <c r="C304" s="112"/>
+      <c r="D304" s="112" t="s">
+        <v>970</v>
+      </c>
+      <c r="E304" s="113" t="s">
+        <v>971</v>
+      </c>
+      <c r="F304" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="G304" s="112"/>
+      <c r="H304" s="104" t="s">
+        <v>761</v>
+      </c>
+      <c r="I304" s="28" t="s">
+        <v>715</v>
+      </c>
+      <c r="J304" s="112"/>
+      <c r="K304" s="27" t="s">
+        <v>337</v>
+      </c>
+      <c r="L304" s="112"/>
+      <c r="M304" s="27" t="s">
+        <v>374</v>
+      </c>
+      <c r="N304" s="114"/>
+      <c r="O304" s="114">
+        <v>2000000144</v>
+      </c>
+      <c r="P304" s="114"/>
+      <c r="Q304" s="28" t="s">
+        <v>369</v>
+      </c>
+      <c r="R304" s="28">
+        <v>9448</v>
+      </c>
+      <c r="S304" s="27" t="s">
+        <v>376</v>
+      </c>
+      <c r="T304" s="114"/>
+      <c r="U304" s="114"/>
+      <c r="V304" s="114"/>
+      <c r="W304" s="114"/>
+      <c r="X304" s="115" t="s">
+        <v>972</v>
+      </c>
     </row>
     <row r="305" spans="7:24">
       <c r="G305" s="23"/>

</xml_diff>

<commit_message>
Fixed bmi to be a measurement
</commit_message>
<xml_diff>
--- a/ncdc_mappings/ncdc_minimal_dataset.xlsx
+++ b/ncdc_mappings/ncdc_minimal_dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Projects/omop-converter/ncdc_mappings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E0FA51E-FDDB-BC4A-B762-F116541C7699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A9CAC1-6E0A-634C-A0E9-51CC71928258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6139,9 +6139,9 @@
   </sheetPr>
   <dimension ref="A1:Y1296"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="90" zoomScaleNormal="89" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U14" sqref="U14"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="89" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M72" sqref="M72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="17"/>
@@ -9510,7 +9510,7 @@
       </c>
       <c r="L71" s="16"/>
       <c r="M71" s="27" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="N71" s="27" t="s">
         <v>368</v>
@@ -9693,7 +9693,7 @@
       </c>
       <c r="L74" s="16"/>
       <c r="M74" s="27" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="N74" s="27" t="s">
         <v>368</v>

</xml_diff>